<commit_message>
paramiters updated,snr numbers limited to 2 dogits
</commit_message>
<xml_diff>
--- a/Khuzestan Network/LINKS.xlsx
+++ b/Khuzestan Network/LINKS.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -172,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,6 +184,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -468,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,11 +535,12 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
+      <c r="H2" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <f>POWER(4.8434, -27)</f>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -561,11 +565,12 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
-        <v>0</v>
+      <c r="H3" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <f t="shared" ref="I3:I38" si="0">POWER(4.8434, -27)</f>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -590,11 +595,12 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1">
-        <v>0</v>
+      <c r="H4" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -619,11 +625,12 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
+      <c r="H5" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -648,11 +655,12 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1">
-        <v>0</v>
+      <c r="H6" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -677,11 +685,12 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1">
-        <v>0</v>
+      <c r="H7" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -706,11 +715,12 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1">
-        <v>0</v>
+      <c r="H8" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -735,11 +745,12 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1">
-        <v>0</v>
+      <c r="H9" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -764,11 +775,12 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1">
-        <v>0</v>
+      <c r="H10" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -793,11 +805,12 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1">
-        <v>0</v>
+      <c r="H11" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -822,11 +835,12 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="1">
-        <v>0</v>
+      <c r="H12" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -851,11 +865,12 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="1">
-        <v>0</v>
+      <c r="H13" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -880,11 +895,12 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1">
-        <v>0</v>
+      <c r="H14" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -909,11 +925,12 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="1">
-        <v>0</v>
+      <c r="H15" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -938,11 +955,12 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="1">
-        <v>0</v>
+      <c r="H16" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -967,11 +985,12 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="1">
-        <v>0</v>
+      <c r="H17" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -996,11 +1015,12 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="1">
-        <v>0</v>
+      <c r="H18" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1025,11 +1045,12 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="H19" s="1">
-        <v>0</v>
+      <c r="H19" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I19" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1054,11 +1075,12 @@
       <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="1">
-        <v>0</v>
+      <c r="H20" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1083,11 +1105,12 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="1">
-        <v>0</v>
+      <c r="H21" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1112,11 +1135,12 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1">
-        <v>0</v>
+      <c r="H22" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1141,11 +1165,12 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
-      <c r="H23" s="1">
-        <v>0</v>
+      <c r="H23" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1170,11 +1195,12 @@
       <c r="G24" s="1">
         <v>0</v>
       </c>
-      <c r="H24" s="1">
-        <v>0</v>
+      <c r="H24" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1199,11 +1225,12 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="1">
-        <v>0</v>
+      <c r="H25" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1228,11 +1255,12 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-      <c r="H26" s="1">
-        <v>0</v>
+      <c r="H26" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I26" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1257,11 +1285,12 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-      <c r="H27" s="1">
-        <v>0</v>
+      <c r="H27" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I27" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1286,11 +1315,12 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="1">
-        <v>0</v>
+      <c r="H28" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I28" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1315,11 +1345,12 @@
       <c r="G29" s="1">
         <v>0</v>
       </c>
-      <c r="H29" s="1">
-        <v>0</v>
+      <c r="H29" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I29" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1344,11 +1375,12 @@
       <c r="G30" s="1">
         <v>0</v>
       </c>
-      <c r="H30" s="1">
-        <v>0</v>
+      <c r="H30" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I30" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1373,11 +1405,12 @@
       <c r="G31" s="1">
         <v>0</v>
       </c>
-      <c r="H31" s="1">
-        <v>0</v>
+      <c r="H31" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I31" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1402,11 +1435,12 @@
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="1">
-        <v>0</v>
+      <c r="H32" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I32" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1431,11 +1465,12 @@
       <c r="G33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="1">
-        <v>0</v>
+      <c r="H33" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I33" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1460,11 +1495,12 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="1">
-        <v>0</v>
+      <c r="H34" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I34" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1489,11 +1525,12 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="1">
-        <v>0</v>
+      <c r="H35" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I35" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1518,11 +1555,12 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-      <c r="H36" s="1">
-        <v>0</v>
+      <c r="H36" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I36" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1547,11 +1585,12 @@
       <c r="G37" s="1">
         <v>0</v>
       </c>
-      <c r="H37" s="1">
-        <v>0</v>
+      <c r="H37" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I37" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1576,11 +1615,12 @@
       <c r="G38" s="1">
         <v>0</v>
       </c>
-      <c r="H38" s="1">
-        <v>0</v>
+      <c r="H38" s="5">
+        <v>1.4E-3</v>
       </c>
       <c r="I38" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
new ui and py file added
</commit_message>
<xml_diff>
--- a/Khuzestan Network/LINKS.xlsx
+++ b/Khuzestan Network/LINKS.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -172,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,9 +184,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -471,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,12 +532,11 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="5">
-        <v>1.4E-3</v>
+      <c r="H2" s="1">
+        <v>0</v>
       </c>
       <c r="I2" s="1">
-        <f>POWER(4.8434, -27)</f>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -565,12 +561,11 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="5">
-        <v>1.4E-3</v>
+      <c r="H3" s="1">
+        <v>0</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I38" si="0">POWER(4.8434, -27)</f>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -595,12 +590,11 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="5">
-        <v>1.4E-3</v>
+      <c r="H4" s="1">
+        <v>0</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -625,12 +619,11 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="5">
-        <v>1.4E-3</v>
+      <c r="H5" s="1">
+        <v>0</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -655,12 +648,11 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="5">
-        <v>1.4E-3</v>
+      <c r="H6" s="1">
+        <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -685,12 +677,11 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="5">
-        <v>1.4E-3</v>
+      <c r="H7" s="1">
+        <v>0</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -715,12 +706,11 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="5">
-        <v>1.4E-3</v>
+      <c r="H8" s="1">
+        <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -745,12 +735,11 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="5">
-        <v>1.4E-3</v>
+      <c r="H9" s="1">
+        <v>0</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -775,12 +764,11 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="5">
-        <v>1.4E-3</v>
+      <c r="H10" s="1">
+        <v>0</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -805,12 +793,11 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="5">
-        <v>1.4E-3</v>
+      <c r="H11" s="1">
+        <v>0</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -835,12 +822,11 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="5">
-        <v>1.4E-3</v>
+      <c r="H12" s="1">
+        <v>0</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -865,12 +851,11 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="5">
-        <v>1.4E-3</v>
+      <c r="H13" s="1">
+        <v>0</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -895,12 +880,11 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="5">
-        <v>1.4E-3</v>
+      <c r="H14" s="1">
+        <v>0</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -925,12 +909,11 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="5">
-        <v>1.4E-3</v>
+      <c r="H15" s="1">
+        <v>0</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -955,12 +938,11 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="5">
-        <v>1.4E-3</v>
+      <c r="H16" s="1">
+        <v>0</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -985,12 +967,11 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="5">
-        <v>1.4E-3</v>
+      <c r="H17" s="1">
+        <v>0</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1015,12 +996,11 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="5">
-        <v>1.4E-3</v>
+      <c r="H18" s="1">
+        <v>0</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1045,12 +1025,11 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="H19" s="5">
-        <v>1.4E-3</v>
+      <c r="H19" s="1">
+        <v>0</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1075,12 +1054,11 @@
       <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="5">
-        <v>1.4E-3</v>
+      <c r="H20" s="1">
+        <v>0</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1105,12 +1083,11 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="5">
-        <v>1.4E-3</v>
+      <c r="H21" s="1">
+        <v>0</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1135,12 +1112,11 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="5">
-        <v>1.4E-3</v>
+      <c r="H22" s="1">
+        <v>0</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1165,12 +1141,11 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
-      <c r="H23" s="5">
-        <v>1.4E-3</v>
+      <c r="H23" s="1">
+        <v>0</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1195,12 +1170,11 @@
       <c r="G24" s="1">
         <v>0</v>
       </c>
-      <c r="H24" s="5">
-        <v>1.4E-3</v>
+      <c r="H24" s="1">
+        <v>0</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1225,12 +1199,11 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="5">
-        <v>1.4E-3</v>
+      <c r="H25" s="1">
+        <v>0</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1255,12 +1228,11 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-      <c r="H26" s="5">
-        <v>1.4E-3</v>
+      <c r="H26" s="1">
+        <v>0</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1285,12 +1257,11 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-      <c r="H27" s="5">
-        <v>1.4E-3</v>
+      <c r="H27" s="1">
+        <v>0</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1315,12 +1286,11 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="5">
-        <v>1.4E-3</v>
+      <c r="H28" s="1">
+        <v>0</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1345,12 +1315,11 @@
       <c r="G29" s="1">
         <v>0</v>
       </c>
-      <c r="H29" s="5">
-        <v>1.4E-3</v>
+      <c r="H29" s="1">
+        <v>0</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1375,12 +1344,11 @@
       <c r="G30" s="1">
         <v>0</v>
       </c>
-      <c r="H30" s="5">
-        <v>1.4E-3</v>
+      <c r="H30" s="1">
+        <v>0</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1405,12 +1373,11 @@
       <c r="G31" s="1">
         <v>0</v>
       </c>
-      <c r="H31" s="5">
-        <v>1.4E-3</v>
+      <c r="H31" s="1">
+        <v>0</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1435,12 +1402,11 @@
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="5">
-        <v>1.4E-3</v>
+      <c r="H32" s="1">
+        <v>0</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1465,12 +1431,11 @@
       <c r="G33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="5">
-        <v>1.4E-3</v>
+      <c r="H33" s="1">
+        <v>0</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1495,12 +1460,11 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="5">
-        <v>1.4E-3</v>
+      <c r="H34" s="1">
+        <v>0</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1525,12 +1489,11 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="5">
-        <v>1.4E-3</v>
+      <c r="H35" s="1">
+        <v>0</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1555,12 +1518,11 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-      <c r="H36" s="5">
-        <v>1.4E-3</v>
+      <c r="H36" s="1">
+        <v>0</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1585,12 +1547,11 @@
       <c r="G37" s="1">
         <v>0</v>
       </c>
-      <c r="H37" s="5">
-        <v>1.4E-3</v>
+      <c r="H37" s="1">
+        <v>0</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1615,12 +1576,11 @@
       <c r="G38" s="1">
         <v>0</v>
       </c>
-      <c r="H38" s="5">
-        <v>1.4E-3</v>
+      <c r="H38" s="1">
+        <v>0</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="0"/>
-        <v>3.169136089868813E-19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>